<commit_message>
Actualización tamaños imágenes rec50
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/SolicitudGrafica_CN_08_04_CO_REC50.xlsx
+++ b/fuentes/contenidos/grado08/guion04/SolicitudGrafica_CN_08_04_CO_REC50.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magda\Desktop\2015\PLANETA\REC_CN_08_04_CO\GRECO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="8895" tabRatio="500"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="196">
   <si>
     <t>Fecha:</t>
   </si>
@@ -559,9 +564,6 @@
     <t>IMG08</t>
   </si>
   <si>
-    <t>CN_08_04_CO_REC50_IMG09.jpg</t>
-  </si>
-  <si>
     <t>Ovulo y espermatozoides</t>
   </si>
   <si>
@@ -580,21 +582,9 @@
     <t>Estrella de mar que representa el proceso de fisión / regeneración</t>
   </si>
   <si>
-    <t>CN_08_04_CO_REC50_IMG10.jpg</t>
-  </si>
-  <si>
-    <t>CN_08_04_CO_REC50_IMG11.jpg</t>
-  </si>
-  <si>
-    <t>CN_08_04_CO_REC50_IMG12.jpg</t>
-  </si>
-  <si>
     <t>CN_08_04_CO_REC50_IMG13.jpg</t>
   </si>
   <si>
-    <t>CN_08_04_CO_REC50_IMG14.jpg</t>
-  </si>
-  <si>
     <t>Ilustración representado el proceso de esporulación</t>
   </si>
   <si>
@@ -635,6 +625,42 @@
   </si>
   <si>
     <t>Avispero, con avispas y larvas</t>
+  </si>
+  <si>
+    <t>800 x 460</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG09n.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG09a.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG10a.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG11a.jpg</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG10n.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG11n.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG12n.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG14n.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_04_CO_REC50_IMG14a.jpg</t>
+  </si>
+  <si>
+    <t>320 x 480</t>
   </si>
 </sst>
 </file>
@@ -1807,7 +1833,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1827,13 +1853,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>590550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1657350</xdr:colOff>
+      <xdr:colOff>1628775</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>1952625</xdr:rowOff>
     </xdr:to>
@@ -1857,7 +1883,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16668750" y="6229350"/>
+          <a:off x="16640175" y="6057900"/>
           <a:ext cx="1333500" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1949,7 +1975,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1957,6 +1983,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1990,7 +2030,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1998,6 +2038,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2031,7 +2085,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2039,6 +2093,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2072,7 +2140,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2080,6 +2148,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2113,7 +2195,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2121,6 +2203,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2154,7 +2250,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2162,6 +2258,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2195,7 +2305,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2203,6 +2313,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2538,9 +2662,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2754,21 +2878,14 @@
       <c r="E10" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="F10" s="75" t="str">
-        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_04_CO_REC50_IMG01.jpg</v>
-      </c>
-      <c r="G10" s="75" t="str">
-        <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
       <c r="H10" s="75" t="str">
         <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I10" s="75" t="str">
-        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG01a.jpg</v>
+      </c>
+      <c r="I10" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J10" s="84" t="s">
         <v>157</v>
@@ -2795,22 +2912,20 @@
       </c>
       <c r="F11" s="75" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_04_CO_REC50_IMG02.jpg</v>
-      </c>
-      <c r="G11" s="75" t="str">
-        <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>CN_08_04_CO_REC50_IMG02n.jpg</v>
+      </c>
+      <c r="G11" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H11" s="75" t="str">
         <f>IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I11" s="75" t="str">
-        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG02a.jpg</v>
+      </c>
+      <c r="I11" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J11" s="68" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="K11" s="70"/>
     </row>
@@ -2833,23 +2948,21 @@
         <v>148</v>
       </c>
       <c r="F12" s="75" t="str">
-        <f t="shared" ref="F12:F17" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A12,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I12="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_04_CO_REC50_IMG03.jpg</v>
-      </c>
-      <c r="G12" s="75" t="str">
-        <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <f t="shared" ref="F12:H17" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A12,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I12="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v>CN_08_04_CO_REC50_IMG03n.jpg</v>
+      </c>
+      <c r="G12" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H12" s="75" t="str">
         <f>IF(AND(I12&lt;&gt;"",I12&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A12,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I12" s="75" t="str">
-        <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG03a.jpg</v>
+      </c>
+      <c r="I12" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J12" s="68" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K12" s="68"/>
     </row>
@@ -2859,7 +2972,7 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="81" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="80" t="str">
         <f t="shared" si="0"/>
@@ -2873,25 +2986,23 @@
       </c>
       <c r="F13" s="75" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_04_CO_REC50_IMG04.jpg</v>
-      </c>
-      <c r="G13" s="75" t="str">
-        <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>CN_08_04_CO_REC50_IMG04n.jpg</v>
+      </c>
+      <c r="G13" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H13" s="75" t="str">
         <f>IF(AND(I13&lt;&gt;"",I13&lt;&gt;0),IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE($C$7,"_",$A13,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I13" s="75" t="str">
-        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG04a.jpg</v>
+      </c>
+      <c r="I13" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J13" s="89" t="s">
+        <v>166</v>
+      </c>
+      <c r="K13" s="73" t="s">
         <v>167</v>
-      </c>
-      <c r="K13" s="73" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="81" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -2899,7 +3010,7 @@
         <v>159</v>
       </c>
       <c r="B14" s="82" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C14" s="80" t="str">
         <f t="shared" si="0"/>
@@ -2913,25 +3024,23 @@
       </c>
       <c r="F14" s="75" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_04_CO_REC50_IMG05.jpg</v>
-      </c>
-      <c r="G14" s="75" t="str">
-        <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>CN_08_04_CO_REC50_IMG05n.jpg</v>
+      </c>
+      <c r="G14" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H14" s="75" t="str">
         <f>IF(AND(I14&lt;&gt;"",I14&lt;&gt;0),IF(OR(B14&lt;&gt;"",J13&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I14" s="75" t="str">
-        <f>IF(OR(B14&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG05a.jpg</v>
+      </c>
+      <c r="I14" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J14" s="90" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K14" s="73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="81" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -2953,26 +3062,24 @@
       </c>
       <c r="F15" s="75" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_04_CO_REC50_IMG06.jpg</v>
-      </c>
-      <c r="G15" s="75" t="str">
-        <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>CN_08_04_CO_REC50_IMG06n.jpg</v>
+      </c>
+      <c r="G15" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H15" s="75" t="str">
         <f>IF(AND(I15&lt;&gt;"",I15&lt;&gt;0),IF(OR(B15&lt;&gt;"",J14&lt;&gt;""),CONCATENATE($C$7,"_",$A15,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I15" s="75" t="str">
-        <f>IF(OR(B15&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG06a.jpg</v>
+      </c>
+      <c r="I15" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J15" s="68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K15" s="69"/>
     </row>
-    <row r="16" spans="1:16" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="81" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A16" s="71" t="s">
         <v>161</v>
       </c>
@@ -2991,22 +3098,20 @@
       </c>
       <c r="F16" s="75" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_04_CO_REC50_IMG07.jpg</v>
-      </c>
-      <c r="G16" s="75" t="str">
-        <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>CN_08_04_CO_REC50_IMG07n.jpg</v>
+      </c>
+      <c r="G16" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H16" s="75" t="str">
         <f>IF(AND(I16&lt;&gt;"",I16&lt;&gt;0),IF(OR(B16&lt;&gt;"",J15&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I16" s="75" t="str">
-        <f>IF(OR(B16&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG07a.jpg</v>
+      </c>
+      <c r="I16" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J16" s="89" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K16" s="69"/>
     </row>
@@ -3027,24 +3132,23 @@
       <c r="E17" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="75" t="str">
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75" t="str">
         <f t="shared" si="1"/>
         <v>CN_08_04_CO_REC50_IMG08.jpg</v>
       </c>
-      <c r="G17" s="75" t="str">
-        <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
+      <c r="I17" s="75" t="s">
+        <v>184</v>
+      </c>
       <c r="J17" s="42" t="s">
         <v>158</v>
       </c>
       <c r="K17" s="69"/>
     </row>
-    <row r="18" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="81" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="74">
         <v>292006460</v>
@@ -3060,23 +3164,23 @@
         <v>148</v>
       </c>
       <c r="F18" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="G18" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="J18" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="75" t="str">
-        <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75" t="str">
-        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="42" t="s">
-        <v>164</v>
-      </c>
       <c r="K18" s="69"/>
     </row>
-    <row r="19" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="81" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A19" s="71" t="s">
         <v>150</v>
       </c>
@@ -3091,22 +3195,22 @@
         <v>147</v>
       </c>
       <c r="E19" s="75" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="F19" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="G19" s="75" t="str">
-        <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75" t="str">
-        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>190</v>
+      </c>
+      <c r="G19" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="H19" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="I19" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J19" s="68" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K19" s="69"/>
     </row>
@@ -3115,7 +3219,7 @@
         <v>151</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C20" s="80" t="str">
         <f t="shared" si="0"/>
@@ -3125,22 +3229,25 @@
         <v>149</v>
       </c>
       <c r="E20" s="75" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="F20" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="G20" s="75" t="str">
-        <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
+        <v>191</v>
+      </c>
+      <c r="G20" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="H20" s="75" t="s">
+        <v>188</v>
+      </c>
+      <c r="I20" s="75" t="s">
+        <v>184</v>
+      </c>
       <c r="J20" s="88" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" s="87" t="s">
         <v>179</v>
-      </c>
-      <c r="K20" s="87" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="81" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3148,7 +3255,7 @@
         <v>152</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C21" s="80" t="str">
         <f t="shared" si="0"/>
@@ -3158,28 +3265,26 @@
         <v>149</v>
       </c>
       <c r="E21" s="75" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="F21" s="75" t="s">
-        <v>172</v>
-      </c>
-      <c r="G21" s="75" t="str">
-        <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>192</v>
+      </c>
+      <c r="G21" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H21" s="75" t="str">
         <f t="shared" ref="H21:H74" si="2">IF(AND(I21&lt;&gt;"",I21&lt;&gt;0),IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE($C$7,"_",$A21,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v/>
-      </c>
-      <c r="I21" s="75" t="str">
-        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG12a.jpg</v>
+      </c>
+      <c r="I21" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J21" s="68" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K21" s="69" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -3200,19 +3305,20 @@
         <v>148</v>
       </c>
       <c r="F22" s="75" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="75" t="str">
-        <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>169</v>
+      </c>
+      <c r="G22" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H22" s="75" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I22" s="75"/>
+        <v>CN_08_04_CO_REC50_IMG13a.jpg</v>
+      </c>
+      <c r="I22" s="75" t="s">
+        <v>184</v>
+      </c>
       <c r="J22" s="68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K22" s="72"/>
     </row>
@@ -3234,28 +3340,31 @@
         <v>148</v>
       </c>
       <c r="F23" s="75" t="s">
-        <v>174</v>
-      </c>
-      <c r="G23" s="75" t="str">
-        <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
+        <v>193</v>
+      </c>
+      <c r="G23" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="I23" s="75" t="s">
+        <v>184</v>
+      </c>
       <c r="J23" s="68" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K23" s="68"/>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="71" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B24" s="91">
         <v>108503651</v>
       </c>
       <c r="C24" s="80" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D24" s="75" t="s">
         <v>147</v>
@@ -3265,22 +3374,20 @@
       </c>
       <c r="F24" s="14" t="str">
         <f t="shared" ref="F24:F74" si="3">IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),CONCATENATE($C$7,"_",$A24,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I24="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_04_CO_REC50_IMG15.jpg</v>
-      </c>
-      <c r="G24" s="14" t="str">
-        <f>IF(F24&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>CN_08_04_CO_REC50_IMG15n.jpg</v>
+      </c>
+      <c r="G24" s="75" t="s">
+        <v>195</v>
       </c>
       <c r="H24" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I24" s="14" t="str">
-        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>CN_08_04_CO_REC50_IMG15a.jpg</v>
+      </c>
+      <c r="I24" s="75" t="s">
+        <v>184</v>
       </c>
       <c r="J24" s="75" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="K24" s="15"/>
     </row>

</xml_diff>